<commit_message>
Fix ComPDF API authentication to use correct OAuth flow
- Update get_compdf_access_token() to use OAuth endpoint with publicKey/secretKey
- Fix all authorization headers to use Bearer access_token instead of publicKey
- Update test_compdf_api.py to use correct authentication flow
- Authentication now works correctly - successfully obtaining access tokens
- Ready for Excel to PDF conversion testing
</commit_message>
<xml_diff>
--- a/temp_uploads/room_classification_140825.xlsx
+++ b/temp_uploads/room_classification_140825.xlsx
@@ -2993,17 +2993,24 @@
           <t xml:space="preserve">EA: </t>
         </is>
       </c>
-      <c r="G38" s="17" t="n"/>
+      <c r="G38" s="17" t="n">
+        <v>74</v>
+      </c>
       <c r="H38" s="45" t="inlineStr">
         <is>
           <t xml:space="preserve">DO: </t>
         </is>
       </c>
-      <c r="I38" s="22" t="n"/>
+      <c r="I38" s="22" t="n">
+        <v>42</v>
+      </c>
       <c r="J38" s="45" t="inlineStr">
         <is>
           <t xml:space="preserve">OD: </t>
         </is>
+      </c>
+      <c r="K38" t="n">
+        <v>32</v>
       </c>
       <c r="L38" s="17" t="n"/>
       <c r="M38" s="22" t="n"/>

</xml_diff>